<commit_message>
màj Docs + création PDFs
</commit_message>
<xml_diff>
--- a/Documentation/Rendu/Journal de travail_MB.xlsx
+++ b/Documentation/Rendu/Journal de travail_MB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\IT2\Projets\MB\TPI\_Rendu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_dev\Shoot4Stats\Documentation\Rendu\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Journal de travail'!$A$1:$I$81</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Journal de travail'!$A$1:$I$82</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
   <si>
     <t>Étude du cahier des charges et création du planning</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Mise en place du projet Vue, adaptation du routage, début 1ère Vue (login)</t>
+  </si>
+  <si>
+    <t>Discussion - faire le point sur l'avancement</t>
   </si>
 </sst>
 </file>
@@ -850,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K82"/>
+  <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -928,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="48">
-        <f>SUM(E8,E14,E21,E28,E44,E51,E60,E77,E81,E31,E66,E69)*24</f>
+        <f>SUM(E8,E14,E22,E29,E45,E52,E61,E78,E82,E32,E67,E70)*24</f>
         <v>24.9</v>
       </c>
       <c r="I5" s="45" t="s">
@@ -1136,7 +1139,7 @@
         <v>5</v>
       </c>
       <c r="E19" s="15">
-        <v>0.64583333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>24</v>
@@ -1145,45 +1148,53 @@
     <row r="20" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="17">
-        <v>0.64583333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="D20" s="24" t="s">
         <v>5</v>
       </c>
       <c r="E20" s="15">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="17">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="15">
         <v>0.70833333333333337</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="2:6" s="29" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="40"/>
-      <c r="C21" s="41" t="s">
+    <row r="22" spans="2:6" s="29" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="40"/>
+      <c r="C22" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="42"/>
-      <c r="E21" s="47">
-        <f>E20-C20+E19-C19+E18-C18+E17-C17</f>
-        <v>0.34375000000000006</v>
-      </c>
-      <c r="F21" s="43"/>
-    </row>
-    <row r="22" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="66">
+      <c r="D22" s="42"/>
+      <c r="E22" s="47">
+        <f>E21-C21+E19-C19+E18-C18+E17-C17+E20-C20</f>
+        <v>0.34375</v>
+      </c>
+      <c r="F22" s="43"/>
+    </row>
+    <row r="23" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="66">
         <v>42828</v>
       </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="10"/>
-    </row>
-    <row r="23" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="9"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="8"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="10"/>
     </row>
     <row r="24" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
@@ -1214,60 +1225,60 @@
       <c r="F27" s="8"/>
     </row>
     <row r="28" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="51"/>
-      <c r="C28" s="52" t="s">
+      <c r="B28" s="9"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="51"/>
+      <c r="C29" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="38"/>
-      <c r="E28" s="46">
-        <f>E27-C27+E26-C26+E25-C25+E24-C24+E23-C23+E22-C22</f>
+      <c r="D29" s="38"/>
+      <c r="E29" s="46">
+        <f>E28-C28+E27-C27+E26-C26+E25-C25+E24-C24+E23-C23</f>
         <v>0</v>
       </c>
-      <c r="F28" s="51"/>
-    </row>
-    <row r="29" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="7">
+      <c r="F29" s="51"/>
+    </row>
+    <row r="30" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="7">
         <v>42829</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="4"/>
-    </row>
-    <row r="30" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="68"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="15"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="14"/>
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="67"/>
-      <c r="C31" s="50" t="s">
+      <c r="B31" s="68"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="67"/>
+      <c r="C32" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="35"/>
-      <c r="E31" s="30">
-        <f>E29-C29+E30-C30</f>
+      <c r="D32" s="35"/>
+      <c r="E32" s="30">
+        <f>E30-C30+E31-C31</f>
         <v>0</v>
       </c>
-      <c r="F31" s="60"/>
-    </row>
-    <row r="32" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="66">
+      <c r="F32" s="60"/>
+    </row>
+    <row r="33" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="66">
         <v>42830</v>
       </c>
-      <c r="C32" s="25"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="54"/>
-    </row>
-    <row r="33" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="9"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="55"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="54"/>
     </row>
     <row r="34" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="9"/>
@@ -1340,45 +1351,45 @@
       <c r="F43" s="55"/>
     </row>
     <row r="44" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="37"/>
-      <c r="C44" s="52" t="s">
+      <c r="B44" s="9"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="55"/>
+    </row>
+    <row r="45" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="37"/>
+      <c r="C45" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="38"/>
-      <c r="E44" s="46">
-        <f>E43-C43+E42-C42+E41-C41+E40-C40+E39-C39+E38-C38+E37-C37+E36-C36+E35-C35+E34-C34+E33-C33+E32-C32</f>
+      <c r="D45" s="38"/>
+      <c r="E45" s="46">
+        <f>E44-C44+E43-C43+E42-C42+E41-C41+E40-C40+E39-C39+E38-C38+E37-C37+E36-C36+E35-C35+E34-C34+E33-C33</f>
         <v>0</v>
       </c>
-      <c r="F44" s="56"/>
-    </row>
-    <row r="45" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="7">
+      <c r="F45" s="56"/>
+    </row>
+    <row r="46" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="7">
         <v>42831</v>
       </c>
-      <c r="C45" s="69" t="s">
+      <c r="C46" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="70"/>
-      <c r="E45" s="71"/>
-      <c r="F45" s="6" t="s">
+      <c r="D46" s="70"/>
+      <c r="E46" s="71"/>
+      <c r="F46" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="66">
+    <row r="47" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="66">
         <v>42832</v>
       </c>
-      <c r="C46" s="25"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="10"/>
-    </row>
-    <row r="47" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="9"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="8"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="10"/>
     </row>
     <row r="48" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="9"/>
@@ -1402,32 +1413,32 @@
       <c r="F50" s="8"/>
     </row>
     <row r="51" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="37"/>
-      <c r="C51" s="52" t="s">
+      <c r="B51" s="9"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="8"/>
+    </row>
+    <row r="52" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="37"/>
+      <c r="C52" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="38"/>
-      <c r="E51" s="46">
-        <f>E50-C50+E49-C49+E48-C48+E47-C47+E46-C46</f>
+      <c r="D52" s="38"/>
+      <c r="E52" s="46">
+        <f>E51-C51+E50-C50+E49-C49+E48-C48+E47-C47</f>
         <v>0</v>
       </c>
-      <c r="F51" s="39"/>
-    </row>
-    <row r="52" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="7">
+      <c r="F52" s="39"/>
+    </row>
+    <row r="53" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="7">
         <v>42835</v>
       </c>
-      <c r="C52" s="16"/>
-      <c r="D52" s="57"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="6"/>
-    </row>
-    <row r="53" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="5"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="4"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="57"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="6"/>
     </row>
     <row r="54" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
@@ -1472,34 +1483,34 @@
       <c r="F59" s="4"/>
     </row>
     <row r="60" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="40"/>
-      <c r="C60" s="58" t="s">
+      <c r="B60" s="5"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="4"/>
+    </row>
+    <row r="61" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="40"/>
+      <c r="C61" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="D60" s="42" t="s">
+      <c r="D61" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="E60" s="47">
-        <f>E59-C59+E58-C58+E57-C57+E56-C56+E55-C55+E54-C54+E53-C53+E52-C52</f>
+      <c r="E61" s="47">
+        <f>E60-C60+E59-C59+E58-C58+E57-C57+E56-C56+E55-C55+E54-C54+E53-C53</f>
         <v>0</v>
       </c>
-      <c r="F60" s="43"/>
-    </row>
-    <row r="61" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="66">
+      <c r="F61" s="43"/>
+    </row>
+    <row r="62" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="66">
         <v>42836</v>
       </c>
-      <c r="C61" s="25"/>
-      <c r="D61" s="53"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="10"/>
-    </row>
-    <row r="62" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="9"/>
-      <c r="C62" s="27"/>
-      <c r="D62" s="22"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="8"/>
+      <c r="C62" s="25"/>
+      <c r="D62" s="53"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="10"/>
     </row>
     <row r="63" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="9"/>
@@ -1523,60 +1534,60 @@
       <c r="F65" s="8"/>
     </row>
     <row r="66" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="37"/>
-      <c r="C66" s="52" t="s">
+      <c r="B66" s="9"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="22"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="8"/>
+    </row>
+    <row r="67" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="37"/>
+      <c r="C67" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D66" s="38"/>
-      <c r="E66" s="46">
-        <f>E65-C65+E64-C64+E63-C63+E62-C62+E61-C61</f>
+      <c r="D67" s="38"/>
+      <c r="E67" s="46">
+        <f>E66-C66+E65-C65+E64-C64+E63-C63+E62-C62</f>
         <v>0</v>
       </c>
-      <c r="F66" s="39"/>
-    </row>
-    <row r="67" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="7">
+      <c r="F67" s="39"/>
+    </row>
+    <row r="68" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="7">
         <v>42835</v>
       </c>
-      <c r="C67" s="16"/>
-      <c r="D67" s="57"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="6"/>
-    </row>
-    <row r="68" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="68"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="15"/>
-      <c r="F68" s="4"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="57"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="6"/>
     </row>
     <row r="69" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="40"/>
-      <c r="C69" s="58" t="s">
+      <c r="B69" s="68"/>
+      <c r="C69" s="17"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="4"/>
+    </row>
+    <row r="70" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="40"/>
+      <c r="C70" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="D69" s="42"/>
-      <c r="E69" s="47">
-        <f>E67-C67+E68-C68</f>
+      <c r="D70" s="42"/>
+      <c r="E70" s="47">
+        <f>E68-C68+E69-C69</f>
         <v>0</v>
       </c>
-      <c r="F69" s="43"/>
-    </row>
-    <row r="70" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="66">
+      <c r="F70" s="43"/>
+    </row>
+    <row r="71" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="66">
         <v>42838</v>
       </c>
-      <c r="C70" s="25"/>
-      <c r="D70" s="53"/>
-      <c r="E70" s="26"/>
-      <c r="F70" s="54"/>
-    </row>
-    <row r="71" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="9"/>
-      <c r="C71" s="27"/>
-      <c r="D71" s="22"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="55"/>
+      <c r="C71" s="25"/>
+      <c r="D71" s="53"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="54"/>
     </row>
     <row r="72" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="9"/>
@@ -1615,31 +1626,31 @@
     </row>
     <row r="77" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="9"/>
-      <c r="C77" s="32" t="s">
+      <c r="C77" s="27"/>
+      <c r="D77" s="22"/>
+      <c r="E77" s="20"/>
+      <c r="F77" s="55"/>
+    </row>
+    <row r="78" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="9"/>
+      <c r="C78" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D77" s="36"/>
-      <c r="E77" s="65">
-        <f>E76-C76+E74-C74+E75-C75+E73-C73+E72-C72+E71-C71+E70-C70</f>
+      <c r="D78" s="36"/>
+      <c r="E78" s="65">
+        <f>E77-C77+E75-C75+E76-C76+E74-C74+E73-C73+E72-C72+E71-C71</f>
         <v>0</v>
       </c>
-      <c r="F77" s="55"/>
-    </row>
-    <row r="78" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="7">
+      <c r="F78" s="55"/>
+    </row>
+    <row r="79" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="7">
         <v>42843</v>
       </c>
-      <c r="C78" s="16"/>
-      <c r="D78" s="57"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="59"/>
-    </row>
-    <row r="79" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="5"/>
-      <c r="C79" s="17"/>
-      <c r="D79" s="24"/>
-      <c r="E79" s="15"/>
-      <c r="F79" s="60"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="57"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="59"/>
     </row>
     <row r="80" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="5"/>
@@ -1649,25 +1660,32 @@
       <c r="F80" s="60"/>
     </row>
     <row r="81" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="63"/>
-      <c r="B81" s="62"/>
-      <c r="C81" s="42" t="s">
+      <c r="B81" s="5"/>
+      <c r="C81" s="17"/>
+      <c r="D81" s="24"/>
+      <c r="E81" s="15"/>
+      <c r="F81" s="60"/>
+    </row>
+    <row r="82" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="63"/>
+      <c r="B82" s="62"/>
+      <c r="C82" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D81" s="42"/>
-      <c r="E81" s="64">
-        <f>E80-C80+E79-C79+E78-C78</f>
+      <c r="D82" s="42"/>
+      <c r="E82" s="64">
+        <f>E81-C81+E80-C80+E79-C79</f>
         <v>0</v>
       </c>
-      <c r="F81" s="61"/>
-    </row>
-    <row r="82" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="24"/>
-      <c r="C82" s="57"/>
+      <c r="F82" s="61"/>
+    </row>
+    <row r="83" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="24"/>
+      <c r="C83" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="H4:I4"/>

</xml_diff>

<commit_message>
doc update + début editShoot
</commit_message>
<xml_diff>
--- a/Documentation/Rendu/Journal de travail_MB.xlsx
+++ b/Documentation/Rendu/Journal de travail_MB.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Journal de travail'!$A$1:$I$82</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Journal de travail'!$A$1:$I$85</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
   <si>
     <t>Étude du cahier des charges et création du planning</t>
   </si>
@@ -123,6 +123,21 @@
   </si>
   <si>
     <t>Rédaction rapport</t>
+  </si>
+  <si>
+    <t>Vue editShoot crée et intégrée / rédaction rapport</t>
+  </si>
+  <si>
+    <t>Visite de l'expert 2 M.Malherbe</t>
+  </si>
+  <si>
+    <t>Mise au point rapport</t>
+  </si>
+  <si>
+    <t>Vue editShoot débutée</t>
+  </si>
+  <si>
+    <t>Discussion avec chef de projet thèmes / selecteur d'Arrow pour editShoot</t>
   </si>
 </sst>
 </file>
@@ -871,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K83"/>
+  <dimension ref="A1:K86"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -949,8 +964,8 @@
         <v>0</v>
       </c>
       <c r="H5" s="48">
-        <f>SUM(E8,E14,E22,E29,E45,E52,E61,E78,E82,E32,E67,E70)*24</f>
-        <v>33.599999999999994</v>
+        <f>SUM(E8,E14,E22,E29,E48,E55,E64,E81,E85,E35,E70,E73)*24</f>
+        <v>42</v>
       </c>
       <c r="I5" s="45" t="s">
         <v>7</v>
@@ -1313,59 +1328,99 @@
       <c r="B30" s="7">
         <v>42829</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="4"/>
+      <c r="C30" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="14">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="31" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="68"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="4"/>
+      <c r="C31" s="17">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="15">
+        <v>0.46875</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="32" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="67"/>
-      <c r="C32" s="50" t="s">
+      <c r="B32" s="68"/>
+      <c r="C32" s="19">
+        <v>0.46875</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F32" s="60" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="68"/>
+      <c r="C33" s="19">
+        <v>0.53125</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="15">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F33" s="60" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="68"/>
+      <c r="C34" s="19">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="15">
+        <v>0.71458333333333324</v>
+      </c>
+      <c r="F34" s="60" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="67"/>
+      <c r="C35" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="30">
-        <f>E30-C30+E31-C31</f>
-        <v>0</v>
-      </c>
-      <c r="F32" s="60"/>
-    </row>
-    <row r="33" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="66">
+      <c r="D35" s="35"/>
+      <c r="E35" s="30">
+        <f>E30-C30+E31-C31+E32-C32+E33-C33+E34-C34</f>
+        <v>0.35</v>
+      </c>
+      <c r="F35" s="60"/>
+    </row>
+    <row r="36" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="66">
         <v>42830</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="54"/>
-    </row>
-    <row r="34" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="9"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="55"/>
-    </row>
-    <row r="35" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="9"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="55"/>
-    </row>
-    <row r="36" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="9"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="55"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="54"/>
     </row>
     <row r="37" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="9"/>
@@ -1424,59 +1479,59 @@
       <c r="F44" s="55"/>
     </row>
     <row r="45" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="37"/>
-      <c r="C45" s="52" t="s">
+      <c r="B45" s="9"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="55"/>
+    </row>
+    <row r="46" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="9"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="55"/>
+    </row>
+    <row r="47" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="9"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="55"/>
+    </row>
+    <row r="48" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="37"/>
+      <c r="C48" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="38"/>
-      <c r="E45" s="46">
-        <f>E44-C44+E43-C43+E42-C42+E41-C41+E40-C40+E39-C39+E38-C38+E37-C37+E36-C36+E35-C35+E34-C34+E33-C33</f>
+      <c r="D48" s="38"/>
+      <c r="E48" s="46">
+        <f>E47-C47+E46-C46+E45-C45+E44-C44+E43-C43+E42-C42+E41-C41+E40-C40+E39-C39+E38-C38+E37-C37+E36-C36</f>
         <v>0</v>
       </c>
-      <c r="F45" s="56"/>
-    </row>
-    <row r="46" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="7">
+      <c r="F48" s="56"/>
+    </row>
+    <row r="49" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="7">
         <v>42831</v>
       </c>
-      <c r="C46" s="69" t="s">
+      <c r="C49" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="D46" s="70"/>
-      <c r="E46" s="71"/>
-      <c r="F46" s="6" t="s">
+      <c r="D49" s="70"/>
+      <c r="E49" s="71"/>
+      <c r="F49" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="66">
+    <row r="50" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="66">
         <v>42832</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="10"/>
-    </row>
-    <row r="48" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="9"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="22"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="8"/>
-    </row>
-    <row r="49" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="9"/>
-      <c r="C49" s="27"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="8"/>
-    </row>
-    <row r="50" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="9"/>
-      <c r="C50" s="27"/>
-      <c r="D50" s="22"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="8"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="10"/>
     </row>
     <row r="51" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="9"/>
@@ -1486,46 +1541,46 @@
       <c r="F51" s="8"/>
     </row>
     <row r="52" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="37"/>
-      <c r="C52" s="52" t="s">
+      <c r="B52" s="9"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="8"/>
+    </row>
+    <row r="53" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="9"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="9"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="8"/>
+    </row>
+    <row r="55" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="37"/>
+      <c r="C55" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="38"/>
-      <c r="E52" s="46">
-        <f>E51-C51+E50-C50+E49-C49+E48-C48+E47-C47</f>
+      <c r="D55" s="38"/>
+      <c r="E55" s="46">
+        <f>E54-C54+E53-C53+E52-C52+E51-C51+E50-C50</f>
         <v>0</v>
       </c>
-      <c r="F52" s="39"/>
-    </row>
-    <row r="53" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="7">
+      <c r="F55" s="39"/>
+    </row>
+    <row r="56" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="7">
         <v>42835</v>
       </c>
-      <c r="C53" s="16"/>
-      <c r="D53" s="57"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="6"/>
-    </row>
-    <row r="54" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="5"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="4"/>
-    </row>
-    <row r="55" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="5"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="4"/>
-    </row>
-    <row r="56" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="5"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="24"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="4"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="57"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="6"/>
     </row>
     <row r="57" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="5"/>
@@ -1556,48 +1611,48 @@
       <c r="F60" s="4"/>
     </row>
     <row r="61" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="40"/>
-      <c r="C61" s="58" t="s">
+      <c r="B61" s="5"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="4"/>
+    </row>
+    <row r="62" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="5"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="4"/>
+    </row>
+    <row r="63" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="5"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="4"/>
+    </row>
+    <row r="64" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="40"/>
+      <c r="C64" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="D61" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="E61" s="47">
-        <f>E60-C60+E59-C59+E58-C58+E57-C57+E56-C56+E55-C55+E54-C54+E53-C53</f>
+      <c r="D64" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" s="47">
+        <f>E63-C63+E62-C62+E61-C61+E60-C60+E59-C59+E58-C58+E57-C57+E56-C56</f>
         <v>0</v>
       </c>
-      <c r="F61" s="43"/>
-    </row>
-    <row r="62" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="66">
+      <c r="F64" s="43"/>
+    </row>
+    <row r="65" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="66">
         <v>42836</v>
       </c>
-      <c r="C62" s="25"/>
-      <c r="D62" s="53"/>
-      <c r="E62" s="26"/>
-      <c r="F62" s="10"/>
-    </row>
-    <row r="63" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="9"/>
-      <c r="C63" s="27"/>
-      <c r="D63" s="22"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="8"/>
-    </row>
-    <row r="64" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="9"/>
-      <c r="C64" s="27"/>
-      <c r="D64" s="22"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="8"/>
-    </row>
-    <row r="65" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="9"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="22"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="8"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="53"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="10"/>
     </row>
     <row r="66" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="9"/>
@@ -1607,74 +1662,74 @@
       <c r="F66" s="8"/>
     </row>
     <row r="67" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="37"/>
-      <c r="C67" s="52" t="s">
+      <c r="B67" s="9"/>
+      <c r="C67" s="27"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="20"/>
+      <c r="F67" s="8"/>
+    </row>
+    <row r="68" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="9"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="20"/>
+      <c r="F68" s="8"/>
+    </row>
+    <row r="69" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="9"/>
+      <c r="C69" s="27"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="8"/>
+    </row>
+    <row r="70" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="37"/>
+      <c r="C70" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D67" s="38"/>
-      <c r="E67" s="46">
-        <f>E66-C66+E65-C65+E64-C64+E63-C63+E62-C62</f>
+      <c r="D70" s="38"/>
+      <c r="E70" s="46">
+        <f>E69-C69+E68-C68+E67-C67+E66-C66+E65-C65</f>
         <v>0</v>
       </c>
-      <c r="F67" s="39"/>
-    </row>
-    <row r="68" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="7">
+      <c r="F70" s="39"/>
+    </row>
+    <row r="71" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="7">
         <v>42835</v>
       </c>
-      <c r="C68" s="16"/>
-      <c r="D68" s="57"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="6"/>
-    </row>
-    <row r="69" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="68"/>
-      <c r="C69" s="17"/>
-      <c r="D69" s="24"/>
-      <c r="E69" s="15"/>
-      <c r="F69" s="4"/>
-    </row>
-    <row r="70" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="40"/>
-      <c r="C70" s="58" t="s">
+      <c r="C71" s="16"/>
+      <c r="D71" s="57"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="6"/>
+    </row>
+    <row r="72" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="68"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="24"/>
+      <c r="E72" s="15"/>
+      <c r="F72" s="4"/>
+    </row>
+    <row r="73" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="40"/>
+      <c r="C73" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="D70" s="42"/>
-      <c r="E70" s="47">
-        <f>E68-C68+E69-C69</f>
+      <c r="D73" s="42"/>
+      <c r="E73" s="47">
+        <f>E71-C71+E72-C72</f>
         <v>0</v>
       </c>
-      <c r="F70" s="43"/>
-    </row>
-    <row r="71" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="66">
+      <c r="F73" s="43"/>
+    </row>
+    <row r="74" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="66">
         <v>42838</v>
       </c>
-      <c r="C71" s="25"/>
-      <c r="D71" s="53"/>
-      <c r="E71" s="26"/>
-      <c r="F71" s="54"/>
-    </row>
-    <row r="72" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="9"/>
-      <c r="C72" s="27"/>
-      <c r="D72" s="22"/>
-      <c r="E72" s="20"/>
-      <c r="F72" s="55"/>
-    </row>
-    <row r="73" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="9"/>
-      <c r="C73" s="27"/>
-      <c r="D73" s="22"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="55"/>
-    </row>
-    <row r="74" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="9"/>
-      <c r="C74" s="27"/>
-      <c r="D74" s="22"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="55"/>
+      <c r="C74" s="25"/>
+      <c r="D74" s="53"/>
+      <c r="E74" s="26"/>
+      <c r="F74" s="54"/>
     </row>
     <row r="75" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="9"/>
@@ -1699,59 +1754,80 @@
     </row>
     <row r="78" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="9"/>
-      <c r="C78" s="32" t="s">
+      <c r="C78" s="27"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="20"/>
+      <c r="F78" s="55"/>
+    </row>
+    <row r="79" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="9"/>
+      <c r="C79" s="27"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="20"/>
+      <c r="F79" s="55"/>
+    </row>
+    <row r="80" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="9"/>
+      <c r="C80" s="27"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="55"/>
+    </row>
+    <row r="81" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="9"/>
+      <c r="C81" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D78" s="36"/>
-      <c r="E78" s="65">
-        <f>E77-C77+E75-C75+E76-C76+E74-C74+E73-C73+E72-C72+E71-C71</f>
+      <c r="D81" s="36"/>
+      <c r="E81" s="65">
+        <f>E80-C80+E78-C78+E79-C79+E77-C77+E76-C76+E75-C75+E74-C74</f>
         <v>0</v>
       </c>
-      <c r="F78" s="55"/>
-    </row>
-    <row r="79" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="7">
+      <c r="F81" s="55"/>
+    </row>
+    <row r="82" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="7">
         <v>42843</v>
       </c>
-      <c r="C79" s="16"/>
-      <c r="D79" s="57"/>
-      <c r="E79" s="14"/>
-      <c r="F79" s="59"/>
-    </row>
-    <row r="80" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="5"/>
-      <c r="C80" s="17"/>
-      <c r="D80" s="24"/>
-      <c r="E80" s="15"/>
-      <c r="F80" s="60"/>
-    </row>
-    <row r="81" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="5"/>
-      <c r="C81" s="17"/>
-      <c r="D81" s="24"/>
-      <c r="E81" s="15"/>
-      <c r="F81" s="60"/>
-    </row>
-    <row r="82" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="63"/>
-      <c r="B82" s="62"/>
-      <c r="C82" s="42" t="s">
+      <c r="C82" s="16"/>
+      <c r="D82" s="57"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="59"/>
+    </row>
+    <row r="83" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="5"/>
+      <c r="C83" s="17"/>
+      <c r="D83" s="24"/>
+      <c r="E83" s="15"/>
+      <c r="F83" s="60"/>
+    </row>
+    <row r="84" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="5"/>
+      <c r="C84" s="17"/>
+      <c r="D84" s="24"/>
+      <c r="E84" s="15"/>
+      <c r="F84" s="60"/>
+    </row>
+    <row r="85" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="63"/>
+      <c r="B85" s="62"/>
+      <c r="C85" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D82" s="42"/>
-      <c r="E82" s="64">
-        <f>E81-C81+E80-C80+E79-C79</f>
+      <c r="D85" s="42"/>
+      <c r="E85" s="64">
+        <f>E84-C84+E83-C83+E82-C82</f>
         <v>0</v>
       </c>
-      <c r="F82" s="61"/>
-    </row>
-    <row r="83" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="24"/>
-      <c r="C83" s="57"/>
+      <c r="F85" s="61"/>
+    </row>
+    <row r="86" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="24"/>
+      <c r="C86" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C49:E49"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="H4:I4"/>

</xml_diff>

<commit_message>
clean code + journal travail
</commit_message>
<xml_diff>
--- a/Documentation/Rendu/Journal de travail_MB.xlsx
+++ b/Documentation/Rendu/Journal de travail_MB.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Journal de travail'!$A$1:$I$85</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Journal de travail'!$A$1:$I$80</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
   <si>
     <t>Étude du cahier des charges et création du planning</t>
   </si>
@@ -138,6 +138,27 @@
   </si>
   <si>
     <t>Discussion avec chef de projet thèmes / selecteur d'Arrow pour editShoot</t>
+  </si>
+  <si>
+    <t>Validation De la vue createShoot</t>
+  </si>
+  <si>
+    <t>Création du composant arrowItem et intégration dans le editShoot</t>
+  </si>
+  <si>
+    <t>Reflexions sur la praticité des ajouts de flèches</t>
+  </si>
+  <si>
+    <t>Mise en place de l'ajout des flèches dans la Vue EditShoot</t>
+  </si>
+  <si>
+    <t>Ajout de paramétres dans la route editShoot pour pas avoir écran blanc à l'actualisation</t>
+  </si>
+  <si>
+    <t>Aide du chef de projet afin d'ordonner les Arrows lors de l'editing</t>
+  </si>
+  <si>
+    <t>Rédaction rapport partie editShoot</t>
   </si>
 </sst>
 </file>
@@ -886,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K86"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44:E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -964,8 +985,8 @@
         <v>0</v>
       </c>
       <c r="H5" s="48">
-        <f>SUM(E8,E14,E22,E29,E48,E55,E64,E81,E85,E35,E70,E73)*24</f>
-        <v>42</v>
+        <f>SUM(E8,E14,E22,E29,E43,E50,E59,E76,E80,E35,E65,E68)*24</f>
+        <v>50.399999999999991</v>
       </c>
       <c r="I5" s="45" t="s">
         <v>7</v>
@@ -1417,170 +1438,226 @@
       <c r="B36" s="66">
         <v>42830</v>
       </c>
-      <c r="C36" s="25"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="54"/>
+      <c r="C36" s="25">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D36" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="26">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F36" s="54" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="37" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="9"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="55"/>
+      <c r="C37" s="27">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="F37" s="55" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="38" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="9"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="55"/>
+      <c r="C38" s="27">
+        <v>0.53125</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="20">
+        <v>0.5625</v>
+      </c>
+      <c r="F38" s="55" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="39" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="9"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="55"/>
-    </row>
-    <row r="40" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="27">
+        <v>0.5625</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="20">
+        <v>0.625</v>
+      </c>
+      <c r="F39" s="55" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="9"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="55"/>
+      <c r="C40" s="27">
+        <v>0.625</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="20">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F40" s="55" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="41" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="9"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="55"/>
+      <c r="C41" s="27">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="20">
+        <v>0.6875</v>
+      </c>
+      <c r="F41" s="55" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="42" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="9"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="55"/>
+      <c r="C42" s="27">
+        <v>0.6875</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="20">
+        <v>0.71458333333333324</v>
+      </c>
+      <c r="F42" s="55" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="43" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="9"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="55"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="38"/>
+      <c r="E43" s="46">
+        <f>E42-C42+E41-C41+E40-C40+E39-C39+E38-C38+E37-C37+E36-C36</f>
+        <v>0.34999999999999992</v>
+      </c>
+      <c r="F43" s="56"/>
     </row>
     <row r="44" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="9"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="55"/>
+      <c r="B44" s="7">
+        <v>42831</v>
+      </c>
+      <c r="C44" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="70"/>
+      <c r="E44" s="71"/>
+      <c r="F44" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="45" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="9"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="55"/>
+      <c r="B45" s="66">
+        <v>42832</v>
+      </c>
+      <c r="C45" s="25"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="10"/>
     </row>
     <row r="46" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="9"/>
       <c r="C46" s="27"/>
       <c r="D46" s="22"/>
       <c r="E46" s="20"/>
-      <c r="F46" s="55"/>
+      <c r="F46" s="8"/>
     </row>
     <row r="47" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="9"/>
       <c r="C47" s="27"/>
       <c r="D47" s="22"/>
       <c r="E47" s="20"/>
-      <c r="F47" s="55"/>
+      <c r="F47" s="8"/>
     </row>
     <row r="48" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="37"/>
-      <c r="C48" s="52" t="s">
+      <c r="B48" s="9"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="8"/>
+    </row>
+    <row r="49" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="9"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="8"/>
+    </row>
+    <row r="50" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="37"/>
+      <c r="C50" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="38"/>
-      <c r="E48" s="46">
-        <f>E47-C47+E46-C46+E45-C45+E44-C44+E43-C43+E42-C42+E41-C41+E40-C40+E39-C39+E38-C38+E37-C37+E36-C36</f>
+      <c r="D50" s="38"/>
+      <c r="E50" s="46">
+        <f>E49-C49+E48-C48+E47-C47+E46-C46+E45-C45</f>
         <v>0</v>
       </c>
-      <c r="F48" s="56"/>
-    </row>
-    <row r="49" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="7">
-        <v>42831</v>
-      </c>
-      <c r="C49" s="69" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" s="70"/>
-      <c r="E49" s="71"/>
-      <c r="F49" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="66">
-        <v>42832</v>
-      </c>
-      <c r="C50" s="25"/>
-      <c r="D50" s="53"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="10"/>
+      <c r="F50" s="39"/>
     </row>
     <row r="51" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="9"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="8"/>
+      <c r="B51" s="7">
+        <v>42835</v>
+      </c>
+      <c r="C51" s="16"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="6"/>
     </row>
     <row r="52" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="9"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="8"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="4"/>
     </row>
     <row r="53" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="9"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="8"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="4"/>
     </row>
     <row r="54" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="9"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="22"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="8"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="4"/>
     </row>
     <row r="55" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="37"/>
-      <c r="C55" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="D55" s="38"/>
-      <c r="E55" s="46">
-        <f>E54-C54+E53-C53+E52-C52+E51-C51+E50-C50</f>
-        <v>0</v>
-      </c>
-      <c r="F55" s="39"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="4"/>
     </row>
     <row r="56" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="7">
-        <v>42835</v>
-      </c>
-      <c r="C56" s="16"/>
-      <c r="D56" s="57"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="6"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="4"/>
     </row>
     <row r="57" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="5"/>
@@ -1597,237 +1674,202 @@
       <c r="F58" s="4"/>
     </row>
     <row r="59" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="5"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="24"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="4"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" s="47">
+        <f>E58-C58+E57-C57+E56-C56+E55-C55+E54-C54+E53-C53+E52-C52+E51-C51</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="43"/>
     </row>
     <row r="60" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="5"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="15"/>
-      <c r="F60" s="4"/>
+      <c r="B60" s="66">
+        <v>42836</v>
+      </c>
+      <c r="C60" s="25"/>
+      <c r="D60" s="53"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="10"/>
     </row>
     <row r="61" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="5"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="15"/>
-      <c r="F61" s="4"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="8"/>
     </row>
     <row r="62" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="5"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="15"/>
-      <c r="F62" s="4"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="27"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="8"/>
     </row>
     <row r="63" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="5"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="24"/>
-      <c r="E63" s="15"/>
-      <c r="F63" s="4"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="20"/>
+      <c r="F63" s="8"/>
     </row>
     <row r="64" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="40"/>
-      <c r="C64" s="58" t="s">
+      <c r="B64" s="9"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="20"/>
+      <c r="F64" s="8"/>
+    </row>
+    <row r="65" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="37"/>
+      <c r="C65" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D64" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="E64" s="47">
-        <f>E63-C63+E62-C62+E61-C61+E60-C60+E59-C59+E58-C58+E57-C57+E56-C56</f>
+      <c r="D65" s="38"/>
+      <c r="E65" s="46">
+        <f>E64-C64+E63-C63+E62-C62+E61-C61+E60-C60</f>
         <v>0</v>
       </c>
-      <c r="F64" s="43"/>
-    </row>
-    <row r="65" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="66">
-        <v>42836</v>
-      </c>
-      <c r="C65" s="25"/>
-      <c r="D65" s="53"/>
-      <c r="E65" s="26"/>
-      <c r="F65" s="10"/>
-    </row>
-    <row r="66" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="9"/>
-      <c r="C66" s="27"/>
-      <c r="D66" s="22"/>
-      <c r="E66" s="20"/>
-      <c r="F66" s="8"/>
-    </row>
-    <row r="67" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="9"/>
-      <c r="C67" s="27"/>
-      <c r="D67" s="22"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="8"/>
-    </row>
-    <row r="68" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="9"/>
-      <c r="C68" s="27"/>
-      <c r="D68" s="22"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="8"/>
-    </row>
-    <row r="69" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="9"/>
-      <c r="C69" s="27"/>
-      <c r="D69" s="22"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="8"/>
-    </row>
-    <row r="70" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="37"/>
-      <c r="C70" s="52" t="s">
+      <c r="F65" s="39"/>
+    </row>
+    <row r="66" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="7">
+        <v>42835</v>
+      </c>
+      <c r="C66" s="16"/>
+      <c r="D66" s="57"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="6"/>
+    </row>
+    <row r="67" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="68"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="4"/>
+    </row>
+    <row r="68" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="40"/>
+      <c r="C68" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="D70" s="38"/>
-      <c r="E70" s="46">
-        <f>E69-C69+E68-C68+E67-C67+E66-C66+E65-C65</f>
+      <c r="D68" s="42"/>
+      <c r="E68" s="47">
+        <f>E66-C66+E67-C67</f>
         <v>0</v>
       </c>
-      <c r="F70" s="39"/>
-    </row>
-    <row r="71" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="7">
-        <v>42835</v>
-      </c>
-      <c r="C71" s="16"/>
-      <c r="D71" s="57"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="6"/>
-    </row>
-    <row r="72" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="68"/>
-      <c r="C72" s="17"/>
-      <c r="D72" s="24"/>
-      <c r="E72" s="15"/>
-      <c r="F72" s="4"/>
-    </row>
-    <row r="73" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="40"/>
-      <c r="C73" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="D73" s="42"/>
-      <c r="E73" s="47">
-        <f>E71-C71+E72-C72</f>
-        <v>0</v>
-      </c>
-      <c r="F73" s="43"/>
-    </row>
-    <row r="74" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="66">
+      <c r="F68" s="43"/>
+    </row>
+    <row r="69" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="66">
         <v>42838</v>
       </c>
-      <c r="C74" s="25"/>
-      <c r="D74" s="53"/>
-      <c r="E74" s="26"/>
-      <c r="F74" s="54"/>
-    </row>
-    <row r="75" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C69" s="25"/>
+      <c r="D69" s="53"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="54"/>
+    </row>
+    <row r="70" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="9"/>
+      <c r="C70" s="27"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="20"/>
+      <c r="F70" s="55"/>
+    </row>
+    <row r="71" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="9"/>
+      <c r="C71" s="27"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="20"/>
+      <c r="F71" s="55"/>
+    </row>
+    <row r="72" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="9"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="20"/>
+      <c r="F72" s="55"/>
+    </row>
+    <row r="73" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="9"/>
+      <c r="C73" s="27"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="20"/>
+      <c r="F73" s="55"/>
+    </row>
+    <row r="74" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="9"/>
+      <c r="C74" s="27"/>
+      <c r="D74" s="22"/>
+      <c r="E74" s="20"/>
+      <c r="F74" s="55"/>
+    </row>
+    <row r="75" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="9"/>
       <c r="C75" s="27"/>
       <c r="D75" s="22"/>
       <c r="E75" s="20"/>
       <c r="F75" s="55"/>
     </row>
-    <row r="76" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="9"/>
-      <c r="C76" s="27"/>
-      <c r="D76" s="22"/>
-      <c r="E76" s="20"/>
+      <c r="C76" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" s="36"/>
+      <c r="E76" s="65">
+        <f>E75-C75+E73-C73+E74-C74+E72-C72+E71-C71+E70-C70+E69-C69</f>
+        <v>0</v>
+      </c>
       <c r="F76" s="55"/>
     </row>
-    <row r="77" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="9"/>
-      <c r="C77" s="27"/>
-      <c r="D77" s="22"/>
-      <c r="E77" s="20"/>
-      <c r="F77" s="55"/>
-    </row>
-    <row r="78" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="9"/>
-      <c r="C78" s="27"/>
-      <c r="D78" s="22"/>
-      <c r="E78" s="20"/>
-      <c r="F78" s="55"/>
-    </row>
-    <row r="79" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="9"/>
-      <c r="C79" s="27"/>
-      <c r="D79" s="22"/>
-      <c r="E79" s="20"/>
-      <c r="F79" s="55"/>
-    </row>
-    <row r="80" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="9"/>
-      <c r="C80" s="27"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="20"/>
-      <c r="F80" s="55"/>
-    </row>
-    <row r="81" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="9"/>
-      <c r="C81" s="32" t="s">
+    <row r="77" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="7">
+        <v>42843</v>
+      </c>
+      <c r="C77" s="16"/>
+      <c r="D77" s="57"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="59"/>
+    </row>
+    <row r="78" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="5"/>
+      <c r="C78" s="17"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="15"/>
+      <c r="F78" s="60"/>
+    </row>
+    <row r="79" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="5"/>
+      <c r="C79" s="17"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="15"/>
+      <c r="F79" s="60"/>
+    </row>
+    <row r="80" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="63"/>
+      <c r="B80" s="62"/>
+      <c r="C80" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D81" s="36"/>
-      <c r="E81" s="65">
-        <f>E80-C80+E78-C78+E79-C79+E77-C77+E76-C76+E75-C75+E74-C74</f>
+      <c r="D80" s="42"/>
+      <c r="E80" s="64">
+        <f>E79-C79+E78-C78+E77-C77</f>
         <v>0</v>
       </c>
-      <c r="F81" s="55"/>
-    </row>
-    <row r="82" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="7">
-        <v>42843</v>
-      </c>
-      <c r="C82" s="16"/>
-      <c r="D82" s="57"/>
-      <c r="E82" s="14"/>
-      <c r="F82" s="59"/>
-    </row>
-    <row r="83" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="5"/>
-      <c r="C83" s="17"/>
-      <c r="D83" s="24"/>
-      <c r="E83" s="15"/>
-      <c r="F83" s="60"/>
-    </row>
-    <row r="84" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="5"/>
-      <c r="C84" s="17"/>
-      <c r="D84" s="24"/>
-      <c r="E84" s="15"/>
-      <c r="F84" s="60"/>
-    </row>
-    <row r="85" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="63"/>
-      <c r="B85" s="62"/>
-      <c r="C85" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="D85" s="42"/>
-      <c r="E85" s="64">
-        <f>E84-C84+E83-C83+E82-C82</f>
-        <v>0</v>
-      </c>
-      <c r="F85" s="61"/>
-    </row>
-    <row r="86" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="24"/>
-      <c r="C86" s="57"/>
+      <c r="F80" s="61"/>
+    </row>
+    <row r="81" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="24"/>
+      <c r="C81" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C44:E44"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="H4:I4"/>

</xml_diff>

<commit_message>
Docs + PDFs update
</commit_message>
<xml_diff>
--- a/Documentation/Rendu/Journal de travail_MB.xlsx
+++ b/Documentation/Rendu/Journal de travail_MB.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="50">
   <si>
     <t>Étude du cahier des charges et création du planning</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Ajout de fonctionnalités ergonomiques niveau editShoot</t>
+  </si>
+  <si>
+    <t>Rédaction rapport + commencement Maquettes</t>
   </si>
 </sst>
 </file>
@@ -925,7 +928,7 @@
   <dimension ref="A1:K82"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1670,7 +1673,7 @@
         <v>0.71458333333333324</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
change menu for ergonomy
</commit_message>
<xml_diff>
--- a/Documentation/Rendu/Journal de travail_MB.xlsx
+++ b/Documentation/Rendu/Journal de travail_MB.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="54">
   <si>
     <t>Étude du cahier des charges et création du planning</t>
   </si>
@@ -177,6 +177,18 @@
   </si>
   <si>
     <t>Rédaction rapport + commencement Maquettes</t>
+  </si>
+  <si>
+    <t>Mise en place d'un EventBus et d'un systéme de "Toast"</t>
+  </si>
+  <si>
+    <t>Fix bug remarqués par testeurs ends négatives</t>
+  </si>
+  <si>
+    <t>Discussion chef de projet structure de données, puis discussion priorité des tâches et enfin desikgn et ergonomie de la partie Archers</t>
+  </si>
+  <si>
+    <t>Gestion de la navbar comme discutée</t>
   </si>
 </sst>
 </file>
@@ -927,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="M54" sqref="M54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1004,7 +1016,7 @@
       </c>
       <c r="H5" s="48">
         <f>SUM(E8,E14,E22,E29,E43,E51,E60,E77,E81,E35,E66,E69)*24</f>
-        <v>58.8</v>
+        <v>62.79999999999999</v>
       </c>
       <c r="I5" s="45" t="s">
         <v>7</v>
@@ -1692,31 +1704,63 @@
       <c r="B52" s="7">
         <v>42835</v>
       </c>
-      <c r="C52" s="16"/>
-      <c r="D52" s="57"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="6"/>
+      <c r="C52" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D52" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="53" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="5"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="4"/>
-    </row>
-    <row r="54" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C53" s="17">
+        <v>0.375</v>
+      </c>
+      <c r="D53" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" s="15">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="4"/>
+      <c r="C54" s="17">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D54" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" s="15">
+        <v>0.46875</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="55" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="4"/>
+      <c r="C55" s="17">
+        <v>0.46875</v>
+      </c>
+      <c r="D55" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="56" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="5"/>
@@ -1756,7 +1800,7 @@
       </c>
       <c r="E60" s="47">
         <f>E59-C59+E58-C58+E57-C57+E56-C56+E55-C55+E54-C54+E53-C53+E52-C52</f>
-        <v>0</v>
+        <v>0.16666666666666669</v>
       </c>
       <c r="F60" s="43"/>
     </row>

</xml_diff>

<commit_message>
stylisation du tableau des points
</commit_message>
<xml_diff>
--- a/Documentation/Rendu/Journal de travail_MB.xlsx
+++ b/Documentation/Rendu/Journal de travail_MB.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="56">
   <si>
     <t>Étude du cahier des charges et création du planning</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>Gestion de la navbar comme discutée</t>
+  </si>
+  <si>
+    <t>Remise en forme VueX + rédaction brève du rapport</t>
+  </si>
+  <si>
+    <t>Stylisation d'editShoot  et des ArrowItems</t>
   </si>
 </sst>
 </file>
@@ -940,7 +946,7 @@
   <dimension ref="A1:K82"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="M54" sqref="M54"/>
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1016,7 +1022,7 @@
       </c>
       <c r="H5" s="48">
         <f>SUM(E8,E14,E22,E29,E43,E51,E60,E77,E81,E35,E66,E69)*24</f>
-        <v>62.79999999999999</v>
+        <v>65.55</v>
       </c>
       <c r="I5" s="45" t="s">
         <v>7</v>
@@ -1764,17 +1770,33 @@
     </row>
     <row r="56" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="5"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="24"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="4"/>
+      <c r="C56" s="17">
+        <v>0.53125</v>
+      </c>
+      <c r="D56" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E56" s="15">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="57" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="5"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="4"/>
+      <c r="C57" s="17">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D57" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E57" s="15">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="58" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="5"/>
@@ -1800,7 +1822,7 @@
       </c>
       <c r="E60" s="47">
         <f>E59-C59+E58-C58+E57-C57+E56-C56+E55-C55+E54-C54+E53-C53+E52-C52</f>
-        <v>0.16666666666666669</v>
+        <v>0.28125000000000006</v>
       </c>
       <c r="F60" s="43"/>
     </row>

</xml_diff>

<commit_message>
add validation for arrows not null
</commit_message>
<xml_diff>
--- a/Documentation/Rendu/Journal de travail_MB.xlsx
+++ b/Documentation/Rendu/Journal de travail_MB.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="59">
   <si>
     <t>Étude du cahier des charges et création du planning</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>Refonte DashBoard</t>
+  </si>
+  <si>
+    <t>Modularisation du code, réflexions sur la partie Archers</t>
   </si>
 </sst>
 </file>
@@ -952,7 +955,7 @@
   <dimension ref="A1:K82"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1028,7 +1031,7 @@
       </c>
       <c r="H5" s="48">
         <f>SUM(E8,E14,E22,E29,E43,E51,E60,E77,E81,E35,E66,E69)*24</f>
-        <v>67.199999999999989</v>
+        <v>69.699999999999989</v>
       </c>
       <c r="I5" s="45" t="s">
         <v>7</v>
@@ -1852,17 +1855,33 @@
       <c r="B61" s="66">
         <v>42836</v>
       </c>
-      <c r="C61" s="25"/>
-      <c r="D61" s="53"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="10"/>
+      <c r="C61" s="25">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D61" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" s="26">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="62" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="9"/>
-      <c r="C62" s="27"/>
-      <c r="D62" s="22"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="8"/>
+      <c r="C62" s="27">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D62" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E62" s="20">
+        <v>0.4375</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="63" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="9"/>
@@ -1893,7 +1912,7 @@
       <c r="D66" s="38"/>
       <c r="E66" s="46">
         <f>E65-C65+E64-C64+E63-C63+E62-C62+E61-C61</f>
-        <v>0</v>
+        <v>0.10416666666666669</v>
       </c>
       <c r="F66" s="39"/>
     </row>

</xml_diff>

<commit_message>
push rapport + docs
</commit_message>
<xml_diff>
--- a/Documentation/Rendu/Journal de travail_MB.xlsx
+++ b/Documentation/Rendu/Journal de travail_MB.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Journal de travail'!$A$1:$I$81</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Journal de travail'!$A$1:$I$87</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="63">
   <si>
     <t>Étude du cahier des charges et création du planning</t>
   </si>
@@ -204,6 +204,18 @@
   </si>
   <si>
     <t>Modularisation du code, réflexions sur la partie Archers</t>
+  </si>
+  <si>
+    <t>Validation dans editShoot en collaboration avec chef de projet (modifs API)</t>
+  </si>
+  <si>
+    <t>Table des points modularisée (ajout dans shootDetails), editShoot petit design</t>
+  </si>
+  <si>
+    <t>Rédaction Rapport</t>
+  </si>
+  <si>
+    <t>Discussion avec Chef de projet, aide sur le design editShoot</t>
   </si>
 </sst>
 </file>
@@ -952,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K82"/>
+  <dimension ref="A1:K88"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1030,8 +1042,8 @@
         <v>0</v>
       </c>
       <c r="H5" s="48">
-        <f>SUM(E8,E14,E22,E29,E43,E51,E60,E77,E81,E35,E66,E69)*24</f>
-        <v>69.699999999999989</v>
+        <f>SUM(E8,E14,E22,E29,E43,E51,E60,E83,E87,E35,E68,E75)*24</f>
+        <v>75.599999999999994</v>
       </c>
       <c r="I5" s="45" t="s">
         <v>7</v>
@@ -1885,167 +1897,249 @@
     </row>
     <row r="63" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="9"/>
-      <c r="C63" s="27"/>
-      <c r="D63" s="22"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="8"/>
+      <c r="C63" s="27">
+        <v>0.4375</v>
+      </c>
+      <c r="D63" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="64" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="9"/>
-      <c r="C64" s="27"/>
-      <c r="D64" s="22"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="8"/>
+      <c r="C64" s="27">
+        <v>0.53125</v>
+      </c>
+      <c r="D64" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" s="20">
+        <v>0.5625</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="65" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="9"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="22"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="8"/>
+      <c r="C65" s="27">
+        <v>0.5625</v>
+      </c>
+      <c r="D65" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" s="20">
+        <v>0.625</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="66" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="37"/>
-      <c r="C66" s="52" t="s">
+      <c r="B66" s="9"/>
+      <c r="C66" s="27">
+        <v>0.625</v>
+      </c>
+      <c r="D66" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E66" s="20">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="9"/>
+      <c r="C67" s="27">
+        <v>0.625</v>
+      </c>
+      <c r="D67" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E67" s="20">
+        <v>0.71458333333333324</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="37"/>
+      <c r="C68" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D66" s="38"/>
-      <c r="E66" s="46">
-        <f>E65-C65+E64-C64+E63-C63+E62-C62+E61-C61</f>
-        <v>0.10416666666666669</v>
-      </c>
-      <c r="F66" s="39"/>
-    </row>
-    <row r="67" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="7">
+      <c r="D68" s="38"/>
+      <c r="E68" s="46">
+        <f>E65-C65+E64-C64+E63-C63+E62-C62+E61-C61+E67-C67</f>
+        <v>0.34999999999999987</v>
+      </c>
+      <c r="F68" s="39"/>
+    </row>
+    <row r="69" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="7">
         <v>42835</v>
       </c>
-      <c r="C67" s="16"/>
-      <c r="D67" s="57"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="6"/>
-    </row>
-    <row r="68" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="68"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="15"/>
-      <c r="F68" s="4"/>
-    </row>
-    <row r="69" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="40"/>
-      <c r="C69" s="58" t="s">
+      <c r="C69" s="16"/>
+      <c r="D69" s="57"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="6"/>
+    </row>
+    <row r="70" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="68"/>
+      <c r="C70" s="17"/>
+      <c r="D70" s="24"/>
+      <c r="E70" s="15"/>
+      <c r="F70" s="4"/>
+    </row>
+    <row r="71" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="68"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="24"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="4"/>
+    </row>
+    <row r="72" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="68"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="24"/>
+      <c r="E72" s="15"/>
+      <c r="F72" s="4"/>
+    </row>
+    <row r="73" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="68"/>
+      <c r="C73" s="17"/>
+      <c r="D73" s="24"/>
+      <c r="E73" s="15"/>
+      <c r="F73" s="4"/>
+    </row>
+    <row r="74" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="68"/>
+      <c r="C74" s="17"/>
+      <c r="D74" s="24"/>
+      <c r="E74" s="15"/>
+      <c r="F74" s="4"/>
+    </row>
+    <row r="75" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="40"/>
+      <c r="C75" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="D69" s="42"/>
-      <c r="E69" s="47">
-        <f>E67-C67+E68-C68</f>
+      <c r="D75" s="42"/>
+      <c r="E75" s="47">
+        <f>E69-C69+E74-C74</f>
         <v>0</v>
       </c>
-      <c r="F69" s="43"/>
-    </row>
-    <row r="70" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="66">
+      <c r="F75" s="43"/>
+    </row>
+    <row r="76" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="66">
         <v>42838</v>
       </c>
-      <c r="C70" s="25"/>
-      <c r="D70" s="53"/>
-      <c r="E70" s="26"/>
-      <c r="F70" s="54"/>
-    </row>
-    <row r="71" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="9"/>
-      <c r="C71" s="27"/>
-      <c r="D71" s="22"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="55"/>
-    </row>
-    <row r="72" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="9"/>
-      <c r="C72" s="27"/>
-      <c r="D72" s="22"/>
-      <c r="E72" s="20"/>
-      <c r="F72" s="55"/>
-    </row>
-    <row r="73" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="9"/>
-      <c r="C73" s="27"/>
-      <c r="D73" s="22"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="55"/>
-    </row>
-    <row r="74" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="9"/>
-      <c r="C74" s="27"/>
-      <c r="D74" s="22"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="55"/>
-    </row>
-    <row r="75" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="9"/>
-      <c r="C75" s="27"/>
-      <c r="D75" s="22"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="55"/>
-    </row>
-    <row r="76" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="9"/>
-      <c r="C76" s="27"/>
-      <c r="D76" s="22"/>
-      <c r="E76" s="20"/>
-      <c r="F76" s="55"/>
+      <c r="C76" s="25"/>
+      <c r="D76" s="53"/>
+      <c r="E76" s="26"/>
+      <c r="F76" s="54"/>
     </row>
     <row r="77" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="9"/>
-      <c r="C77" s="32" t="s">
+      <c r="C77" s="27"/>
+      <c r="D77" s="22"/>
+      <c r="E77" s="20"/>
+      <c r="F77" s="55"/>
+    </row>
+    <row r="78" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="9"/>
+      <c r="C78" s="27"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="20"/>
+      <c r="F78" s="55"/>
+    </row>
+    <row r="79" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="9"/>
+      <c r="C79" s="27"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="20"/>
+      <c r="F79" s="55"/>
+    </row>
+    <row r="80" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="9"/>
+      <c r="C80" s="27"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="55"/>
+    </row>
+    <row r="81" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="9"/>
+      <c r="C81" s="27"/>
+      <c r="D81" s="22"/>
+      <c r="E81" s="20"/>
+      <c r="F81" s="55"/>
+    </row>
+    <row r="82" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="9"/>
+      <c r="C82" s="27"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="20"/>
+      <c r="F82" s="55"/>
+    </row>
+    <row r="83" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="9"/>
+      <c r="C83" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D77" s="36"/>
-      <c r="E77" s="65">
-        <f>E76-C76+E74-C74+E75-C75+E73-C73+E72-C72+E71-C71+E70-C70</f>
+      <c r="D83" s="36"/>
+      <c r="E83" s="65">
+        <f>E82-C82+E80-C80+E81-C81+E79-C79+E78-C78+E77-C77+E76-C76</f>
         <v>0</v>
       </c>
-      <c r="F77" s="55"/>
-    </row>
-    <row r="78" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="7">
+      <c r="F83" s="55"/>
+    </row>
+    <row r="84" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="7">
         <v>42843</v>
       </c>
-      <c r="C78" s="16"/>
-      <c r="D78" s="57"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="59"/>
-    </row>
-    <row r="79" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="5"/>
-      <c r="C79" s="17"/>
-      <c r="D79" s="24"/>
-      <c r="E79" s="15"/>
-      <c r="F79" s="60"/>
-    </row>
-    <row r="80" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="5"/>
-      <c r="C80" s="17"/>
-      <c r="D80" s="24"/>
-      <c r="E80" s="15"/>
-      <c r="F80" s="60"/>
-    </row>
-    <row r="81" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="63"/>
-      <c r="B81" s="62"/>
-      <c r="C81" s="42" t="s">
+      <c r="C84" s="16"/>
+      <c r="D84" s="57"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="59"/>
+    </row>
+    <row r="85" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="5"/>
+      <c r="C85" s="17"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="15"/>
+      <c r="F85" s="60"/>
+    </row>
+    <row r="86" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="5"/>
+      <c r="C86" s="17"/>
+      <c r="D86" s="24"/>
+      <c r="E86" s="15"/>
+      <c r="F86" s="60"/>
+    </row>
+    <row r="87" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="63"/>
+      <c r="B87" s="62"/>
+      <c r="C87" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D81" s="42"/>
-      <c r="E81" s="64">
-        <f>E80-C80+E79-C79+E78-C78</f>
+      <c r="D87" s="42"/>
+      <c r="E87" s="64">
+        <f>E86-C86+E85-C85+E84-C84</f>
         <v>0</v>
       </c>
-      <c r="F81" s="61"/>
-    </row>
-    <row r="82" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="24"/>
-      <c r="C82" s="57"/>
+      <c r="F87" s="61"/>
+    </row>
+    <row r="88" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="24"/>
+      <c r="C88" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Add shootMapper to fix bug at shootCreation
</commit_message>
<xml_diff>
--- a/Documentation/Rendu/Journal de travail_MB.xlsx
+++ b/Documentation/Rendu/Journal de travail_MB.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Journal de travail'!$A$1:$I$87</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Journal de travail'!$A$1:$I$90</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="72">
   <si>
     <t>Étude du cahier des charges et création du planning</t>
   </si>
@@ -216,6 +216,33 @@
   </si>
   <si>
     <t>Discussion avec Chef de projet, aide sur le design editShoot</t>
+  </si>
+  <si>
+    <t>Modification de l'API afin de compter les flèches de chaque point</t>
+  </si>
+  <si>
+    <t>Modularisation de VueX</t>
+  </si>
+  <si>
+    <t>VueX ajout user et shoots</t>
+  </si>
+  <si>
+    <t>Ajout d'un systéme de  toaster avec erreur ou succés</t>
+  </si>
+  <si>
+    <t>stylisation DashBoard</t>
+  </si>
+  <si>
+    <t>stylisation EditShoot</t>
+  </si>
+  <si>
+    <t>add Shoot avec VueX avec l'aide du chef de projet</t>
+  </si>
+  <si>
+    <t>Petites stylisations sur les pages don’t page Home</t>
+  </si>
+  <si>
+    <t>Essais de stylisation sur une liste avec chef de projet</t>
   </si>
 </sst>
 </file>
@@ -964,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K88"/>
+  <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1042,8 +1069,8 @@
         <v>0</v>
       </c>
       <c r="H5" s="48">
-        <f>SUM(E8,E14,E22,E29,E43,E51,E60,E83,E87,E35,E68,E75)*24</f>
-        <v>75.599999999999994</v>
+        <f>SUM(E8,E14,E22,E29,E43,E51,E60,E86,E90,E35,E68,E78)*24</f>
+        <v>86.499999999999986</v>
       </c>
       <c r="I5" s="45" t="s">
         <v>7</v>
@@ -1986,87 +2013,167 @@
       <c r="B69" s="7">
         <v>42835</v>
       </c>
-      <c r="C69" s="16"/>
-      <c r="D69" s="57"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="6"/>
+      <c r="C69" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D69" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="E69" s="14">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="70" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="68"/>
-      <c r="C70" s="17"/>
-      <c r="D70" s="24"/>
-      <c r="E70" s="15"/>
-      <c r="F70" s="4"/>
+      <c r="C70" s="17">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D70" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70" s="15">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="71" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="68"/>
-      <c r="C71" s="17"/>
-      <c r="D71" s="24"/>
-      <c r="E71" s="15"/>
-      <c r="F71" s="4"/>
+      <c r="C71" s="17">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D71" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E71" s="15">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="72" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="68"/>
-      <c r="C72" s="17"/>
-      <c r="D72" s="24"/>
-      <c r="E72" s="15"/>
-      <c r="F72" s="4"/>
+      <c r="C72" s="17">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D72" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E72" s="15">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="73" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="68"/>
-      <c r="C73" s="17"/>
-      <c r="D73" s="24"/>
-      <c r="E73" s="15"/>
-      <c r="F73" s="4"/>
+      <c r="C73" s="17">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D73" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E73" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="74" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="68"/>
-      <c r="C74" s="17"/>
-      <c r="D74" s="24"/>
-      <c r="E74" s="15"/>
-      <c r="F74" s="4"/>
+      <c r="C74" s="17">
+        <v>0.53125</v>
+      </c>
+      <c r="D74" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E74" s="15">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="75" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="40"/>
-      <c r="C75" s="58" t="s">
+      <c r="B75" s="68"/>
+      <c r="C75" s="17">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="D75" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E75" s="15">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="68"/>
+      <c r="C76" s="17">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="D76" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E76" s="15">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="68"/>
+      <c r="C77" s="17">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D77" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E77" s="15">
+        <v>0.75624999999999998</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="40"/>
+      <c r="C78" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="D75" s="42"/>
-      <c r="E75" s="47">
-        <f>E69-C69+E74-C74</f>
-        <v>0</v>
-      </c>
-      <c r="F75" s="43"/>
-    </row>
-    <row r="76" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="66">
+      <c r="D78" s="42"/>
+      <c r="E78" s="47">
+        <f>E69-C69+E77-C77+E70-C70+E71-C71+E72-C72+E73-C73+E74-C74+E75-C75+E76-C76</f>
+        <v>0.39166666666666661</v>
+      </c>
+      <c r="F78" s="43"/>
+    </row>
+    <row r="79" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="66">
         <v>42838</v>
       </c>
-      <c r="C76" s="25"/>
-      <c r="D76" s="53"/>
-      <c r="E76" s="26"/>
-      <c r="F76" s="54"/>
-    </row>
-    <row r="77" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="9"/>
-      <c r="C77" s="27"/>
-      <c r="D77" s="22"/>
-      <c r="E77" s="20"/>
-      <c r="F77" s="55"/>
-    </row>
-    <row r="78" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="9"/>
-      <c r="C78" s="27"/>
-      <c r="D78" s="22"/>
-      <c r="E78" s="20"/>
-      <c r="F78" s="55"/>
-    </row>
-    <row r="79" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="9"/>
-      <c r="C79" s="27"/>
-      <c r="D79" s="22"/>
-      <c r="E79" s="20"/>
-      <c r="F79" s="55"/>
+      <c r="C79" s="25">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D79" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E79" s="26">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F79" s="54" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="80" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="9"/>
@@ -2091,55 +2198,76 @@
     </row>
     <row r="83" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="9"/>
-      <c r="C83" s="32" t="s">
+      <c r="C83" s="27"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="20"/>
+      <c r="F83" s="55"/>
+    </row>
+    <row r="84" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="9"/>
+      <c r="C84" s="27"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="20"/>
+      <c r="F84" s="55"/>
+    </row>
+    <row r="85" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="9"/>
+      <c r="C85" s="27"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="20"/>
+      <c r="F85" s="55"/>
+    </row>
+    <row r="86" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="9"/>
+      <c r="C86" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D83" s="36"/>
-      <c r="E83" s="65">
-        <f>E82-C82+E80-C80+E81-C81+E79-C79+E78-C78+E77-C77+E76-C76</f>
+      <c r="D86" s="36"/>
+      <c r="E86" s="65">
+        <f>E85-C85+E83-C83+E84-C84+E82-C82+E81-C81+E80-C80+E79-C79</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F86" s="55"/>
+    </row>
+    <row r="87" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="7">
+        <v>42843</v>
+      </c>
+      <c r="C87" s="16"/>
+      <c r="D87" s="57"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="59"/>
+    </row>
+    <row r="88" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="5"/>
+      <c r="C88" s="17"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="15"/>
+      <c r="F88" s="60"/>
+    </row>
+    <row r="89" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="5"/>
+      <c r="C89" s="17"/>
+      <c r="D89" s="24"/>
+      <c r="E89" s="15"/>
+      <c r="F89" s="60"/>
+    </row>
+    <row r="90" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="63"/>
+      <c r="B90" s="62"/>
+      <c r="C90" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D90" s="42"/>
+      <c r="E90" s="64">
+        <f>E89-C89+E88-C88+E87-C87</f>
         <v>0</v>
       </c>
-      <c r="F83" s="55"/>
-    </row>
-    <row r="84" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="7">
-        <v>42843</v>
-      </c>
-      <c r="C84" s="16"/>
-      <c r="D84" s="57"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="59"/>
-    </row>
-    <row r="85" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="5"/>
-      <c r="C85" s="17"/>
-      <c r="D85" s="24"/>
-      <c r="E85" s="15"/>
-      <c r="F85" s="60"/>
-    </row>
-    <row r="86" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="5"/>
-      <c r="C86" s="17"/>
-      <c r="D86" s="24"/>
-      <c r="E86" s="15"/>
-      <c r="F86" s="60"/>
-    </row>
-    <row r="87" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="63"/>
-      <c r="B87" s="62"/>
-      <c r="C87" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="D87" s="42"/>
-      <c r="E87" s="64">
-        <f>E86-C86+E85-C85+E84-C84</f>
-        <v>0</v>
-      </c>
-      <c r="F87" s="61"/>
-    </row>
-    <row r="88" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="24"/>
-      <c r="C88" s="57"/>
+      <c r="F90" s="61"/>
+    </row>
+    <row r="91" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="24"/>
+      <c r="C91" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
fix add arrow at editShoot
</commit_message>
<xml_diff>
--- a/Documentation/Rendu/Journal de travail_MB.xlsx
+++ b/Documentation/Rendu/Journal de travail_MB.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Journal de travail'!$A$1:$I$88</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Journal de travail'!$A$1:$I$89</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="76">
   <si>
     <t>Étude du cahier des charges et création du planning</t>
   </si>
@@ -248,10 +248,13 @@
     <t>Stylisation et ajout d'un graphique dans ShootDetails</t>
   </si>
   <si>
-    <t>Discussion avec chef de projet afin de faire le point et voir satisfaction travail accompli</t>
-  </si>
-  <si>
     <t>Rédaction rapport conception ajout outils et ressources</t>
+  </si>
+  <si>
+    <t>Discussion avec chef de projet afin de faire le point et voir reste du travail</t>
+  </si>
+  <si>
+    <t>Petites stylisations afin de rendre l'appli nette</t>
   </si>
 </sst>
 </file>
@@ -1000,10 +1003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K89"/>
+  <dimension ref="A1:K90"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="H90" sqref="H90"/>
+      <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1081,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="48">
-        <f>SUM(E8,E14,E22,E29,E43,E51,E60,E84,E88,E35,E68,E78)*24</f>
+        <f>SUM(E8,E14,E22,E29,E43,E51,E60,E85,E89,E35,E68,E78)*24</f>
         <v>93.149999999999991</v>
       </c>
       <c r="I5" s="45" t="s">
@@ -2020,7 +2023,7 @@
     </row>
     <row r="69" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="7">
-        <v>42835</v>
+        <v>42837</v>
       </c>
       <c r="C69" s="16">
         <v>0.33333333333333331</v>
@@ -2226,10 +2229,10 @@
         <v>0.625</v>
       </c>
       <c r="F82" s="55" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="9"/>
       <c r="C83" s="27">
         <v>0.625</v>
@@ -2238,39 +2241,47 @@
         <v>5</v>
       </c>
       <c r="E83" s="20">
+        <v>0.65625</v>
+      </c>
+      <c r="F83" s="55" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="9"/>
+      <c r="C84" s="27">
+        <v>0.65625</v>
+      </c>
+      <c r="D84" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E84" s="20">
         <v>0.67291666666666661</v>
       </c>
-      <c r="F83" s="55" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="9"/>
-      <c r="C84" s="32" t="s">
+      <c r="F84" s="55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="9"/>
+      <c r="C85" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D84" s="36"/>
-      <c r="E84" s="65">
-        <f>+E83-C83+E82-C82+E81-C81+E80-C80+E79-C79</f>
+      <c r="D85" s="36"/>
+      <c r="E85" s="65">
+        <f>E83-C83+E84-C84+E82-C82+E81-C81+E80-C80+E79-C79</f>
         <v>0.33958333333333329</v>
       </c>
-      <c r="F84" s="55"/>
-    </row>
-    <row r="85" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="7">
+      <c r="F85" s="55"/>
+    </row>
+    <row r="86" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="7">
         <v>42843</v>
       </c>
-      <c r="C85" s="16"/>
-      <c r="D85" s="57"/>
-      <c r="E85" s="14"/>
-      <c r="F85" s="59"/>
-    </row>
-    <row r="86" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="5"/>
-      <c r="C86" s="17"/>
-      <c r="D86" s="24"/>
-      <c r="E86" s="15"/>
-      <c r="F86" s="60"/>
+      <c r="C86" s="16"/>
+      <c r="D86" s="57"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="59"/>
     </row>
     <row r="87" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="5"/>
@@ -2280,21 +2291,28 @@
       <c r="F87" s="60"/>
     </row>
     <row r="88" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="63"/>
-      <c r="B88" s="62"/>
-      <c r="C88" s="42" t="s">
+      <c r="B88" s="5"/>
+      <c r="C88" s="17"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="15"/>
+      <c r="F88" s="60"/>
+    </row>
+    <row r="89" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="63"/>
+      <c r="B89" s="62"/>
+      <c r="C89" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D88" s="42"/>
-      <c r="E88" s="64">
-        <f>E87-C87+E86-C86+E85-C85</f>
+      <c r="D89" s="42"/>
+      <c r="E89" s="64">
+        <f>E88-C88+E87-C87+E86-C86</f>
         <v>0</v>
       </c>
-      <c r="F88" s="61"/>
-    </row>
-    <row r="89" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="24"/>
-      <c r="C89" s="57"/>
+      <c r="F89" s="61"/>
+    </row>
+    <row r="90" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="24"/>
+      <c r="C90" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>